<commit_message>
more excel files .. additional attempts lp
</commit_message>
<xml_diff>
--- a/data/cl_planned_schedule - good option 1.xlsx
+++ b/data/cl_planned_schedule - good option 1.xlsx
@@ -8,14 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/667b39c49d6998ed/Documents/cl_schedule/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B7567EFC11C337E3880827363A688FD24B1E3255" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D7F730-1899-43D4-A6DB-6E9A4E4F6A08}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_B7567EFC11C337E3880827363A688FD24B1E3255" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC09DEB7-4D2B-4805-82F4-B727A9C44DDF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cl_shifts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cl_shifts!$A$1:$I$81</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -143,9 +158,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,12 +210,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,18 +557,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +584,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -582,94 +597,98 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3">
+        <v>44743</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <f>MATCH(F2,F:F)</f>
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2">
-        <v>44746</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2">
-        <v>44747</v>
+        <v>19</v>
+      </c>
+      <c r="F3" s="3">
+        <v>44744</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44748</v>
+        <v>19</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44745</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -685,11 +704,11 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
-        <v>44749</v>
+      <c r="F5" s="3">
+        <v>44746</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -698,7 +717,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -714,11 +733,11 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2">
-        <v>44750</v>
+      <c r="F6" s="3">
+        <v>44747</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
@@ -727,169 +746,169 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44748</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2">
-        <v>44753</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2">
-        <v>44754</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44749</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
         <v>37</v>
       </c>
       <c r="I8">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2">
-        <v>44755</v>
+        <v>13</v>
+      </c>
+      <c r="F9" s="3">
+        <v>44750</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
       </c>
       <c r="I9">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2">
-        <v>44756</v>
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44751</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2">
-        <v>44757</v>
+        <v>20</v>
+      </c>
+      <c r="F11" s="3">
+        <v>44752</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I11">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="2">
-        <v>44760</v>
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
+        <v>44753</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -898,27 +917,27 @@
         <v>37</v>
       </c>
       <c r="I12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="2">
-        <v>44761</v>
+        <v>14</v>
+      </c>
+      <c r="F13" s="3">
+        <v>44754</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -927,27 +946,27 @@
         <v>37</v>
       </c>
       <c r="I13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44762</v>
+        <v>14</v>
+      </c>
+      <c r="F14" s="3">
+        <v>44755</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -956,27 +975,27 @@
         <v>37</v>
       </c>
       <c r="I14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="2">
-        <v>44763</v>
+        <v>14</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44756</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -985,27 +1004,27 @@
         <v>37</v>
       </c>
       <c r="I15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2">
-        <v>44764</v>
+        <v>14</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44757</v>
       </c>
       <c r="G16">
         <v>6</v>
@@ -1014,27 +1033,27 @@
         <v>37</v>
       </c>
       <c r="I16">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2">
-        <v>44779</v>
+        <v>32</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44758</v>
       </c>
       <c r="G17">
         <v>7</v>
@@ -1043,27 +1062,27 @@
         <v>38</v>
       </c>
       <c r="I17">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="2">
-        <v>44780</v>
+        <v>32</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44759</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1072,7 +1091,7 @@
         <v>38</v>
       </c>
       <c r="I18">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1080,28 +1099,28 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="2">
-        <v>44800</v>
+        <v>15</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44760</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1109,28 +1128,28 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2">
-        <v>44801</v>
+        <v>15</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44761</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1138,28 +1157,28 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="2">
-        <v>44807</v>
+        <v>15</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44762</v>
       </c>
       <c r="G21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1167,115 +1186,115 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="2">
-        <v>44808</v>
+        <v>15</v>
+      </c>
+      <c r="F22" s="3">
+        <v>44763</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="2">
-        <v>44744</v>
+        <v>15</v>
+      </c>
+      <c r="F23" s="3">
+        <v>44764</v>
       </c>
       <c r="G23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="2">
-        <v>44745</v>
+        <v>25</v>
+      </c>
+      <c r="F24" s="3">
+        <v>44765</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
       </c>
       <c r="I24">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="2">
-        <v>44751</v>
+        <v>25</v>
+      </c>
+      <c r="F25" s="3">
+        <v>44766</v>
       </c>
       <c r="G25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
       </c>
       <c r="I25">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1283,28 +1302,28 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="2">
-        <v>44752</v>
+        <v>21</v>
+      </c>
+      <c r="F26" s="3">
+        <v>44767</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1323,11 +1342,11 @@
       <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="2">
-        <v>44767</v>
+      <c r="F27" s="3">
+        <v>44768</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
         <v>37</v>
@@ -1352,11 +1371,11 @@
       <c r="E28" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="2">
-        <v>44768</v>
+      <c r="F28" s="3">
+        <v>44769</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>37</v>
@@ -1381,11 +1400,11 @@
       <c r="E29" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="2">
-        <v>44769</v>
+      <c r="F29" s="3">
+        <v>44770</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
@@ -1410,11 +1429,11 @@
       <c r="E30" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="2">
-        <v>44770</v>
+      <c r="F30" s="3">
+        <v>44771</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" t="s">
         <v>37</v>
@@ -1425,28 +1444,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="2">
-        <v>44771</v>
+        <v>26</v>
+      </c>
+      <c r="F31" s="3">
+        <v>44772</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I31">
         <v>31</v>
@@ -1454,379 +1473,379 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="2">
-        <v>44788</v>
+        <v>26</v>
+      </c>
+      <c r="F32" s="3">
+        <v>44773</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I32">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B33">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="2">
-        <v>44789</v>
+        <v>33</v>
+      </c>
+      <c r="F33" s="3">
+        <v>44774</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
       <c r="I33">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B34">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34" s="2">
-        <v>44790</v>
+        <v>33</v>
+      </c>
+      <c r="F34" s="3">
+        <v>44775</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34" t="s">
         <v>37</v>
       </c>
       <c r="I34">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B35">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="2">
-        <v>44791</v>
+        <v>33</v>
+      </c>
+      <c r="F35" s="3">
+        <v>44776</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H35" t="s">
         <v>37</v>
       </c>
       <c r="I35">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="2">
-        <v>44792</v>
+        <v>33</v>
+      </c>
+      <c r="F36" s="3">
+        <v>44777</v>
       </c>
       <c r="G36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H36" t="s">
         <v>37</v>
       </c>
       <c r="I36">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B37">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="2">
-        <v>44795</v>
+        <v>33</v>
+      </c>
+      <c r="F37" s="3">
+        <v>44778</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H37" t="s">
         <v>37</v>
       </c>
       <c r="I37">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
         <v>16</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>16</v>
-      </c>
-      <c r="E38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="2">
-        <v>44796</v>
+      <c r="F38" s="3">
+        <v>44779</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I38">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
         <v>16</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>16</v>
-      </c>
-      <c r="E39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="2">
-        <v>44797</v>
+      <c r="F39" s="3">
+        <v>44780</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I39">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B40">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="2">
-        <v>44798</v>
+        <v>34</v>
+      </c>
+      <c r="F40" s="3">
+        <v>44781</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
         <v>37</v>
       </c>
       <c r="I40">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B41">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="2">
-        <v>44799</v>
+        <v>34</v>
+      </c>
+      <c r="F41" s="3">
+        <v>44782</v>
       </c>
       <c r="G41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H41" t="s">
         <v>37</v>
       </c>
       <c r="I41">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B42">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="2">
-        <v>44821</v>
+        <v>34</v>
+      </c>
+      <c r="F42" s="3">
+        <v>44783</v>
       </c>
       <c r="G42">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I42">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B43">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="2">
-        <v>44822</v>
+        <v>34</v>
+      </c>
+      <c r="F43" s="3">
+        <v>44784</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I43">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="2">
-        <v>44765</v>
+        <v>34</v>
+      </c>
+      <c r="F44" s="3">
+        <v>44785</v>
       </c>
       <c r="G44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I44">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -1834,28 +1853,28 @@
         <v>11</v>
       </c>
       <c r="B45">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="3">
+        <v>44786</v>
+      </c>
+      <c r="G45">
         <v>7</v>
       </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>7</v>
-      </c>
-      <c r="E45" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="2">
-        <v>44766</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
       <c r="H45" t="s">
         <v>38</v>
       </c>
       <c r="I45">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -1863,112 +1882,112 @@
         <v>11</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="2">
-        <v>44772</v>
+        <v>27</v>
+      </c>
+      <c r="F46" s="3">
+        <v>44787</v>
       </c>
       <c r="G46">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H46" t="s">
         <v>38</v>
       </c>
       <c r="I46">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="2">
-        <v>44773</v>
+        <v>22</v>
+      </c>
+      <c r="F47" s="3">
+        <v>44788</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I47">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="2">
-        <v>44786</v>
+        <v>22</v>
+      </c>
+      <c r="F48" s="3">
+        <v>44789</v>
       </c>
       <c r="G48">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I48">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="2">
-        <v>44787</v>
+        <v>22</v>
+      </c>
+      <c r="F49" s="3">
+        <v>44790</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I49">
         <v>34</v>
@@ -1976,28 +1995,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
-      </c>
-      <c r="F50" s="2">
-        <v>44793</v>
+        <v>22</v>
+      </c>
+      <c r="F50" s="3">
+        <v>44791</v>
       </c>
       <c r="G50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I50">
         <v>34</v>
@@ -2005,31 +2024,31 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>28</v>
-      </c>
-      <c r="F51" s="2">
-        <v>44794</v>
+        <v>22</v>
+      </c>
+      <c r="F51" s="3">
+        <v>44792</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I51">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -2037,28 +2056,28 @@
         <v>11</v>
       </c>
       <c r="B52">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F52" s="2">
-        <v>44809</v>
+        <v>28</v>
+      </c>
+      <c r="F52" s="3">
+        <v>44793</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I52">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -2066,260 +2085,260 @@
         <v>11</v>
       </c>
       <c r="B53">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F53" s="2">
-        <v>44810</v>
+        <v>28</v>
+      </c>
+      <c r="F53" s="3">
+        <v>44794</v>
       </c>
       <c r="G53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I53">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54" s="2">
-        <v>44811</v>
+        <v>23</v>
+      </c>
+      <c r="F54" s="3">
+        <v>44795</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H54" t="s">
         <v>37</v>
       </c>
       <c r="I54">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E55" t="s">
-        <v>29</v>
-      </c>
-      <c r="F55" s="2">
-        <v>44812</v>
+        <v>23</v>
+      </c>
+      <c r="F55" s="3">
+        <v>44796</v>
       </c>
       <c r="G55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H55" t="s">
         <v>37</v>
       </c>
       <c r="I55">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
-      </c>
-      <c r="F56" s="2">
-        <v>44813</v>
+        <v>23</v>
+      </c>
+      <c r="F56" s="3">
+        <v>44797</v>
       </c>
       <c r="G56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H56" t="s">
         <v>37</v>
       </c>
       <c r="I56">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="2">
-        <v>44816</v>
+        <v>23</v>
+      </c>
+      <c r="F57" s="3">
+        <v>44798</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H57" t="s">
         <v>37</v>
       </c>
       <c r="I57">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="2">
-        <v>44817</v>
+        <v>23</v>
+      </c>
+      <c r="F58" s="3">
+        <v>44799</v>
       </c>
       <c r="G58">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H58" t="s">
         <v>37</v>
       </c>
       <c r="I58">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>30</v>
-      </c>
-      <c r="F59" s="2">
-        <v>44818</v>
+        <v>17</v>
+      </c>
+      <c r="F59" s="3">
+        <v>44800</v>
       </c>
       <c r="G59">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I59">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>30</v>
-      </c>
-      <c r="F60" s="2">
-        <v>44819</v>
+        <v>17</v>
+      </c>
+      <c r="F60" s="3">
+        <v>44801</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I60">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E61" t="s">
-        <v>30</v>
-      </c>
-      <c r="F61" s="2">
-        <v>44820</v>
+        <v>35</v>
+      </c>
+      <c r="F61" s="3">
+        <v>44802</v>
       </c>
       <c r="G61">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H61" t="s">
         <v>37</v>
       </c>
       <c r="I61">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -2327,28 +2346,28 @@
         <v>12</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E62" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" s="2">
-        <v>44743</v>
+        <v>35</v>
+      </c>
+      <c r="F62" s="3">
+        <v>44803</v>
       </c>
       <c r="G62">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H62" t="s">
         <v>37</v>
       </c>
       <c r="I62">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2356,28 +2375,28 @@
         <v>12</v>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E63" t="s">
-        <v>32</v>
-      </c>
-      <c r="F63" s="2">
-        <v>44758</v>
+        <v>35</v>
+      </c>
+      <c r="F63" s="3">
+        <v>44804</v>
       </c>
       <c r="G63">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I63">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2385,28 +2404,28 @@
         <v>12</v>
       </c>
       <c r="B64">
+        <v>18</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>18</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="3">
+        <v>44805</v>
+      </c>
+      <c r="G64">
         <v>5</v>
       </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64">
-        <v>5</v>
-      </c>
-      <c r="E64" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="2">
-        <v>44759</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
       <c r="H64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I64">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -2414,231 +2433,231 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E65" t="s">
-        <v>33</v>
-      </c>
-      <c r="F65" s="2">
-        <v>44774</v>
+        <v>35</v>
+      </c>
+      <c r="F65" s="3">
+        <v>44806</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H65" t="s">
         <v>37</v>
       </c>
       <c r="I65">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B66">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E66" t="s">
-        <v>33</v>
-      </c>
-      <c r="F66" s="2">
-        <v>44775</v>
+        <v>18</v>
+      </c>
+      <c r="F66" s="3">
+        <v>44807</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H66" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I66">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E67" t="s">
-        <v>33</v>
-      </c>
-      <c r="F67" s="2">
-        <v>44776</v>
+        <v>18</v>
+      </c>
+      <c r="F67" s="3">
+        <v>44808</v>
       </c>
       <c r="G67">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I67">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="2">
-        <v>44777</v>
+        <v>29</v>
+      </c>
+      <c r="F68" s="3">
+        <v>44809</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H68" t="s">
         <v>37</v>
       </c>
       <c r="I68">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B69">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" s="2">
-        <v>44778</v>
+        <v>29</v>
+      </c>
+      <c r="F69" s="3">
+        <v>44810</v>
       </c>
       <c r="G69">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H69" t="s">
         <v>37</v>
       </c>
       <c r="I69">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E70" t="s">
-        <v>34</v>
-      </c>
-      <c r="F70" s="2">
-        <v>44781</v>
+        <v>29</v>
+      </c>
+      <c r="F70" s="3">
+        <v>44811</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H70" t="s">
         <v>37</v>
       </c>
       <c r="I70">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E71" t="s">
-        <v>34</v>
-      </c>
-      <c r="F71" s="2">
-        <v>44782</v>
+        <v>29</v>
+      </c>
+      <c r="F71" s="3">
+        <v>44812</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H71" t="s">
         <v>37</v>
       </c>
       <c r="I71">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E72" t="s">
-        <v>34</v>
-      </c>
-      <c r="F72" s="2">
-        <v>44783</v>
+        <v>29</v>
+      </c>
+      <c r="F72" s="3">
+        <v>44813</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H72" t="s">
         <v>37</v>
       </c>
       <c r="I72">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -2646,28 +2665,28 @@
         <v>12</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E73" t="s">
-        <v>34</v>
-      </c>
-      <c r="F73" s="2">
-        <v>44784</v>
+        <v>36</v>
+      </c>
+      <c r="F73" s="3">
+        <v>44814</v>
       </c>
       <c r="G73">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H73" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I73">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -2675,48 +2694,48 @@
         <v>12</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E74" t="s">
-        <v>34</v>
-      </c>
-      <c r="F74" s="2">
-        <v>44785</v>
+        <v>36</v>
+      </c>
+      <c r="F74" s="3">
+        <v>44815</v>
       </c>
       <c r="G74">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I74">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E75" t="s">
-        <v>35</v>
-      </c>
-      <c r="F75" s="2">
-        <v>44802</v>
+        <v>30</v>
+      </c>
+      <c r="F75" s="3">
+        <v>44816</v>
       </c>
       <c r="G75">
         <v>2</v>
@@ -2725,27 +2744,27 @@
         <v>37</v>
       </c>
       <c r="I75">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B76">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E76" t="s">
-        <v>35</v>
-      </c>
-      <c r="F76" s="2">
-        <v>44803</v>
+        <v>30</v>
+      </c>
+      <c r="F76" s="3">
+        <v>44817</v>
       </c>
       <c r="G76">
         <v>3</v>
@@ -2754,27 +2773,27 @@
         <v>37</v>
       </c>
       <c r="I76">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E77" t="s">
-        <v>35</v>
-      </c>
-      <c r="F77" s="2">
-        <v>44804</v>
+        <v>30</v>
+      </c>
+      <c r="F77" s="3">
+        <v>44818</v>
       </c>
       <c r="G77">
         <v>4</v>
@@ -2783,27 +2802,27 @@
         <v>37</v>
       </c>
       <c r="I77">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E78" t="s">
-        <v>35</v>
-      </c>
-      <c r="F78" s="2">
-        <v>44805</v>
+        <v>30</v>
+      </c>
+      <c r="F78" s="3">
+        <v>44819</v>
       </c>
       <c r="G78">
         <v>5</v>
@@ -2812,27 +2831,27 @@
         <v>37</v>
       </c>
       <c r="I78">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E79" t="s">
-        <v>35</v>
-      </c>
-      <c r="F79" s="2">
-        <v>44806</v>
+        <v>30</v>
+      </c>
+      <c r="F79" s="3">
+        <v>44820</v>
       </c>
       <c r="G79">
         <v>6</v>
@@ -2841,27 +2860,27 @@
         <v>37</v>
       </c>
       <c r="I79">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B80">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E80" t="s">
-        <v>36</v>
-      </c>
-      <c r="F80" s="2">
-        <v>44814</v>
+        <v>24</v>
+      </c>
+      <c r="F80" s="3">
+        <v>44821</v>
       </c>
       <c r="G80">
         <v>7</v>
@@ -2870,27 +2889,27 @@
         <v>38</v>
       </c>
       <c r="I80">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E81" t="s">
-        <v>36</v>
-      </c>
-      <c r="F81" s="2">
-        <v>44815</v>
+        <v>24</v>
+      </c>
+      <c r="F81" s="3">
+        <v>44822</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -2899,10 +2918,16 @@
         <v>38</v>
       </c>
       <c r="I81">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I81" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I81">
+      <sortCondition ref="F1:F81"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>